<commit_message>
Updates to Audio progress notes
</commit_message>
<xml_diff>
--- a/Music/(UpToDate) Stuart Audio Asset List.xlsx
+++ b/Music/(UpToDate) Stuart Audio Asset List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="122">
   <si>
     <t>NAME</t>
   </si>
@@ -156,9 +156,6 @@
   </si>
   <si>
     <t>Bubbles too quickly and at too high a pitch; pitch down and reduce speed. Think beans or curry bubbling?</t>
-  </si>
-  <si>
-    <t>Just needs better note-choice, to make for more musical transitions/cadence</t>
   </si>
   <si>
     <t>Perfect for now, will need to do some editing when animation is complete, likely have more of a fade-in?</t>
@@ -368,6 +365,54 @@
   </si>
   <si>
     <t>Far Eastern/Asian Tropes</t>
+  </si>
+  <si>
+    <t>Now the music slows down in speed with the current music track as it transitions between planes, I just need to get the speed right to sync with the game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fire Burning </t>
+  </si>
+  <si>
+    <t>Boulder Rolling</t>
+  </si>
+  <si>
+    <t>Ogre Grunts</t>
+  </si>
+  <si>
+    <t>Progress Noise</t>
+  </si>
+  <si>
+    <t>UI Navigation</t>
+  </si>
+  <si>
+    <t>Ambient burning w/Low pass</t>
+  </si>
+  <si>
+    <t>To warn player it's a danger</t>
+  </si>
+  <si>
+    <t>Charging Ogre Aggressive</t>
+  </si>
+  <si>
+    <t>When player places key platform</t>
+  </si>
+  <si>
+    <t>Typical Chiptune Nav</t>
+  </si>
+  <si>
+    <t>Aztec Ambience</t>
+  </si>
+  <si>
+    <t>Eastern Ambience</t>
+  </si>
+  <si>
+    <t>Egyptian Ambience</t>
+  </si>
+  <si>
+    <t>Natural sounds to accompany ST</t>
+  </si>
+  <si>
+    <t>To be layered behind the 3 plane soundtracks, in order to phase in between planes with the same functionality (avoids more programming)</t>
   </si>
 </sst>
 </file>
@@ -783,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,12 +839,12 @@
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="18.140625" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="133.5703125" customWidth="1"/>
+    <col min="9" max="9" width="135.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -836,7 +881,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
         <v>31</v>
@@ -848,10 +893,10 @@
         <v>33</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H3" t="s">
         <v>37</v>
@@ -862,22 +907,22 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
@@ -888,22 +933,22 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H5" t="s">
         <v>37</v>
@@ -914,19 +959,19 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>34</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>36</v>
@@ -943,19 +988,19 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>34</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>36</v>
@@ -972,19 +1017,19 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>34</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>36</v>
@@ -1001,19 +1046,19 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>36</v>
@@ -1027,19 +1072,19 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>36</v>
@@ -1053,19 +1098,19 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>36</v>
@@ -1079,13 +1124,13 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>33</v>
@@ -1105,13 +1150,13 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>33</v>
@@ -1131,13 +1176,13 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>34</v>
@@ -1160,13 +1205,13 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>33</v>
@@ -1186,13 +1231,13 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>33</v>
@@ -1209,16 +1254,16 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>33</v>
@@ -1238,13 +1283,13 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>35</v>
@@ -1259,7 +1304,7 @@
         <v>41</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1267,13 +1312,13 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>33</v>
@@ -1281,11 +1326,14 @@
       <c r="F19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>36</v>
+      <c r="G19" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="H19" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1293,28 +1341,28 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>36</v>
+        <v>49</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="H20" t="s">
-        <v>74</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>44</v>
+        <v>73</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1322,28 +1370,28 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>36</v>
+        <v>49</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="H21" t="s">
-        <v>74</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>44</v>
+        <v>73</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1351,13 +1399,13 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>35</v>
@@ -1372,7 +1420,7 @@
         <v>37</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1380,13 +1428,13 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>33</v>
@@ -1406,13 +1454,13 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>33</v>
@@ -1432,13 +1480,13 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>33</v>
@@ -1455,16 +1503,16 @@
     </row>
     <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="B26" t="s">
-        <v>100</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>35</v>
@@ -1476,24 +1524,24 @@
         <v>36</v>
       </c>
       <c r="H26" t="s">
+        <v>60</v>
+      </c>
+      <c r="I26" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>33</v>
@@ -1507,19 +1555,22 @@
       <c r="H27" t="s">
         <v>38</v>
       </c>
+      <c r="I27" s="6" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>33</v>
@@ -1533,43 +1584,49 @@
       <c r="H28" t="s">
         <v>38</v>
       </c>
+      <c r="I28" s="6" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>36</v>
+        <v>91</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="H29" t="s">
         <v>38</v>
       </c>
+      <c r="I29" s="6" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>33</v>
@@ -1577,23 +1634,26 @@
       <c r="F30" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>36</v>
+      <c r="G30" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="H30" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>33</v>
@@ -1601,23 +1661,26 @@
       <c r="F31" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G31" s="3" t="s">
-        <v>36</v>
+      <c r="G31" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="H31" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>33</v>
@@ -1625,23 +1688,26 @@
       <c r="F32" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G32" s="3" t="s">
-        <v>36</v>
+      <c r="G32" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="H32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>33</v>
@@ -1649,23 +1715,26 @@
       <c r="F33" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G33" s="3" t="s">
-        <v>36</v>
+      <c r="G33" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="H33" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>33</v>
@@ -1673,23 +1742,26 @@
       <c r="F34" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G34" s="3" t="s">
-        <v>36</v>
+      <c r="G34" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="H34" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>33</v>
@@ -1697,11 +1769,174 @@
       <c r="F35" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G35" s="3" t="s">
-        <v>36</v>
+      <c r="G35" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="H35" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>117</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>119</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>